<commit_message>
Aggiornato Avanzamento.xlsx da lbianco via Streamlit
</commit_message>
<xml_diff>
--- a/Avanzamento.xlsx
+++ b/Avanzamento.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,7 +508,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="3">
-        <f>C2-(C2*D2)/100</f>
+        <f t="shared" ref="E2:E25" si="0">C2-(C2*D2)/100</f>
         <v>28.207999999999998</v>
       </c>
     </row>
@@ -526,7 +526,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="3">
-        <f>C3-(C3*D3)/100</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
@@ -544,7 +544,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="3">
-        <f>C4-(C4*D4)/100</f>
+        <f t="shared" si="0"/>
         <v>37.6</v>
       </c>
     </row>
@@ -562,7 +562,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="3">
-        <f>C5-(C5*D5)/100</f>
+        <f t="shared" si="0"/>
         <v>28.256</v>
       </c>
     </row>
@@ -580,7 +580,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="3">
-        <f>C6-(C6*D6)/100</f>
+        <f t="shared" si="0"/>
         <v>33.016000000000005</v>
       </c>
     </row>
@@ -598,7 +598,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="3">
-        <f>C7-(C7*D7)/100</f>
+        <f t="shared" si="0"/>
         <v>25.936</v>
       </c>
     </row>
@@ -616,7 +616,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="3">
-        <f>C8-(C8*D8)/100</f>
+        <f t="shared" si="0"/>
         <v>13.247999999999999</v>
       </c>
     </row>
@@ -634,7 +634,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="3">
-        <f>C9-(C9*D9)/100</f>
+        <f t="shared" si="0"/>
         <v>21.84</v>
       </c>
     </row>
@@ -652,7 +652,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="3">
-        <f>C10-(C10*D10)/100</f>
+        <f t="shared" si="0"/>
         <v>22.608000000000001</v>
       </c>
     </row>
@@ -670,7 +670,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="3">
-        <f>C11-(C11*D11)/100</f>
+        <f t="shared" si="0"/>
         <v>28.792000000000002</v>
       </c>
     </row>
@@ -688,7 +688,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="3">
-        <f>C12-(C12*D12)/100</f>
+        <f t="shared" si="0"/>
         <v>26.96</v>
       </c>
     </row>
@@ -706,7 +706,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="3">
-        <f>C13-(C13*D13)/100</f>
+        <f t="shared" si="0"/>
         <v>31.463999999999999</v>
       </c>
     </row>
@@ -724,7 +724,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="3">
-        <f>C14-(C14*D14)/100</f>
+        <f t="shared" si="0"/>
         <v>25.856000000000002</v>
       </c>
     </row>
@@ -742,7 +742,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="3">
-        <f>C15-(C15*D15)/100</f>
+        <f t="shared" si="0"/>
         <v>25.6</v>
       </c>
     </row>
@@ -760,7 +760,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="3">
-        <f>C16-(C16*D16)/100</f>
+        <f t="shared" si="0"/>
         <v>31.463999999999999</v>
       </c>
     </row>
@@ -778,7 +778,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="3">
-        <f>C17-(C17*D17)/100</f>
+        <f t="shared" si="0"/>
         <v>25.6</v>
       </c>
     </row>
@@ -796,7 +796,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="3">
-        <f>C18-(C18*D18)/100</f>
+        <f t="shared" si="0"/>
         <v>23.047999999999998</v>
       </c>
     </row>
@@ -814,7 +814,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="3">
-        <f>C19-(C19*D19)/100</f>
+        <f t="shared" si="0"/>
         <v>26.048000000000002</v>
       </c>
     </row>
@@ -832,7 +832,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="3">
-        <f>C20-(C20*D20)/100</f>
+        <f t="shared" si="0"/>
         <v>30.032</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="3">
-        <f>C21-(C21*D21)/100</f>
+        <f t="shared" si="0"/>
         <v>26.439999999999998</v>
       </c>
     </row>
@@ -868,7 +868,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="3">
-        <f>C22-(C22*D22)/100</f>
+        <f t="shared" si="0"/>
         <v>28.256</v>
       </c>
     </row>
@@ -886,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="3">
-        <f>C23-(C23*D23)/100</f>
+        <f t="shared" si="0"/>
         <v>23.872</v>
       </c>
     </row>
@@ -898,14 +898,14 @@
         <v>88</v>
       </c>
       <c r="C24" s="4">
-        <v>35.99</v>
+        <v>35</v>
       </c>
       <c r="D24" s="6">
         <v>20</v>
       </c>
       <c r="E24" s="3">
-        <f>C24-(C24*D24)/100</f>
-        <v>28.792000000000002</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -922,7 +922,7 @@
         <v>20</v>
       </c>
       <c r="E25" s="3">
-        <f>C25-(C25*D25)/100</f>
+        <f t="shared" si="0"/>
         <v>33.463999999999999</v>
       </c>
     </row>

</xml_diff>